<commit_message>
creating time basers (us)
</commit_message>
<xml_diff>
--- a/timer_period_calculation.xlsx
+++ b/timer_period_calculation.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\Documents\Curso STM32\MCU2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D50179B-FF5A-4FC3-9893-24A63EBA03CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="7230"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -57,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,12 +121,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -154,7 +171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,9 +204,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,6 +256,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,11 +448,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>4999</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -438,7 +489,7 @@
       </c>
       <c r="B8">
         <f>B4/(B6+1)</f>
-        <v>10000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -447,7 +498,7 @@
       </c>
       <c r="B10">
         <f>1/B8</f>
-        <v>1E-4</v>
+        <v>1.9999999999999999E-7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -456,7 +507,7 @@
       </c>
       <c r="B12">
         <f>B14/B10</f>
-        <v>10000</v>
+        <v>50.000000000000007</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -517,7 +568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -529,7 +580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>